<commit_message>
More local config changes
</commit_message>
<xml_diff>
--- a/Quiz Questions.xlsx
+++ b/Quiz Questions.xlsx
@@ -82,7 +82,7 @@
   <si>
     <t xml:space="preserve">Foo
 Bar
-Fizz
+Chocolate
 Buzz</t>
   </si>
 </sst>
@@ -238,7 +238,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>